<commit_message>
Caught a typo in column header
</commit_message>
<xml_diff>
--- a/build-presets/Energy-yield_deg-rates.xlsx
+++ b/build-presets/Energy-yield_deg-rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bsmith5/WebLCOE-master/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABD9AC5-E8E9-F443-9A89-835256AAAB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793D25D6-C490-6B4C-A3BF-C2B2F9DE56E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13160" yWindow="2220" windowWidth="25240" windowHeight="18880" xr2:uid="{2516EB6E-C874-8B4C-B15F-B97A9FB825A3}"/>
+    <workbookView xWindow="16460" yWindow="1920" windowWidth="18300" windowHeight="18880" xr2:uid="{2516EB6E-C874-8B4C-B15F-B97A9FB825A3}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="8" r:id="rId1"/>
@@ -224,10 +224,10 @@
     <t>Cell Technology</t>
   </si>
   <si>
-    <t>Package Typ</t>
+    <t>System Type</t>
   </si>
   <si>
-    <t>System Type</t>
+    <t>Package Type</t>
   </si>
 </sst>
 </file>
@@ -633,16 +633,18 @@
   <dimension ref="A1:G601"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F723" sqref="F723"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="39.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -650,10 +652,10 @@
         <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>

</xml_diff>